<commit_message>
Voting + option 2 window 3 on new autoencoded data
</commit_message>
<xml_diff>
--- a/data/performance_sheets_option2/window3/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets_option2/window3/BA11 Overall Model Peformance Results.xlsx
@@ -1158,23 +1158,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.006227677175367666</v>
+        <v>0.009787880571043081</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.07013242974191913</v>
+        <v>0.08038319242361527</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1062673906100404</v>
+        <v>0.1278157895554757</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.0789156332760985</v>
+        <v>0.0989337180694382</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>10.90199362828113</v>
+        <v>14.19676046850967</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -1188,23 +1188,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.01608510843851662</v>
+        <v>0.009422136052502991</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.104348050773825</v>
+        <v>0.07726740787296153</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.1424720266133005</v>
+        <v>0.1227596072587556</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1268270808562454</v>
+        <v>0.09706768799401266</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>15.68331394110732</v>
+        <v>13.737014321248</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -1220,53 +1220,53 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.0441042734127546</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.1589638857013131</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.2397721136383145</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.2100101745457934</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>31.05648664390132</v>
+      </c>
+      <c r="I14" s="9" t="inlineStr">
+        <is>
+          <t>Stacking Regressor</t>
+        </is>
+      </c>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
           <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
-      <c r="D14" s="5" t="n">
-        <v>0.01489863495618776</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>0.08572824752604997</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0.104670410818723</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>0.1220599645919486</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>11.30172288333299</v>
-      </c>
-      <c r="I14" s="9" t="inlineStr">
-        <is>
-          <t>Stacking Regressor</t>
-        </is>
-      </c>
-      <c r="J14" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K14" s="8" t="inlineStr">
-        <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
-        </is>
-      </c>
       <c r="L14" s="8" t="n">
-        <v>0.01108360571677216</v>
+        <v>0.01303412229023363</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.08157643177187199</v>
+        <v>0.08988830492123773</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.1030539664908283</v>
+        <v>0.1404809928818966</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.1052787049539087</v>
+        <v>0.1141670805890806</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>10.87957181592384</v>
+        <v>16.33109308765422</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -1286,19 +1286,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.005371818388721027</v>
+        <v>0.03609552827482029</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.05767740574874389</v>
+        <v>0.1514746517063751</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.0799552755491689</v>
+        <v>0.2173384776164657</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.07329268987232647</v>
+        <v>0.1899882319377184</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>8.242399149206877</v>
+        <v>25.95341647370845</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -1312,23 +1312,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.0287968940377449</v>
+        <v>0.02346536627353878</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1346694674264526</v>
+        <v>0.1231892297575184</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.1807014839804815</v>
+        <v>0.1911711494254131</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.16969647620898</v>
+        <v>0.1531840927561957</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>20.79699699605062</v>
+        <v>20.81026678334928</v>
       </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
@@ -2477,19 +2477,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.3712623836817053</v>
+        <v>1.891773839498786</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.535995317601343</v>
+        <v>1.232868304968821</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1988071971106411</v>
+        <v>0.5084056762071291</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.6093130424352537</v>
+        <v>1.375417696374009</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>22.75601659450721</v>
+        <v>64.10498996654314</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -2503,23 +2503,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.5726248538104205</v>
+        <v>1.657848903343636</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.5669907676172303</v>
+        <v>1.064458810729928</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2143476801936829</v>
+        <v>0.4271969111190322</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.7567197987435115</v>
+        <v>1.287574814658797</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>25.38794835383396</v>
+        <v>56.07874391799395</v>
       </c>
     </row>
     <row r="14">
@@ -2535,53 +2535,53 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.4906824581497126</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.521461517983722</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.2913494761951105</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.7004873004913883</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>21.70300777453182</v>
+      </c>
+      <c r="I14" s="9" t="inlineStr">
+        <is>
+          <t>Stacking Regressor</t>
+        </is>
+      </c>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
           <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
-      <c r="D14" s="5" t="n">
-        <v>0.532100764337331</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>0.5836875253965723</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0.2474587641747181</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>0.7294523729054084</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>23.84981237919986</v>
-      </c>
-      <c r="I14" s="9" t="inlineStr">
-        <is>
-          <t>Stacking Regressor</t>
-        </is>
-      </c>
-      <c r="J14" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K14" s="8" t="inlineStr">
-        <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
-        </is>
-      </c>
       <c r="L14" s="8" t="n">
-        <v>0.655415993035116</v>
+        <v>0.3503491522275282</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.607100075991142</v>
+        <v>0.4465830634994993</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.263442810125734</v>
+        <v>0.247274236525233</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.809577663374624</v>
+        <v>0.5919029922441077</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>20.71458375227469</v>
+        <v>19.05506545301107</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -2597,23 +2597,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.2203574033619524</v>
+        <v>0.2928421714273323</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3921286815384012</v>
+        <v>0.4483091867219979</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.1609170221671404</v>
+        <v>0.2250696128974493</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.4694224146352115</v>
+        <v>0.541148936455882</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>16.58729868738146</v>
+        <v>19.26246633374114</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -2631,19 +2631,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.2124637645268565</v>
+        <v>0.301412982126994</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.3649543474081371</v>
+        <v>0.4569552253660787</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.1592807351830235</v>
+        <v>0.2283517694415798</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.4609379183001291</v>
+        <v>0.5490109125755097</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>14.73924744293366</v>
+        <v>19.60917220627816</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -3785,53 +3785,53 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.9209023664943535</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.7782320631669662</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.28486690971801</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.9596365804273791</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>36.63924911123164</v>
+      </c>
+      <c r="I13" s="9" t="inlineStr">
+        <is>
+          <t>Voting Regressor</t>
+        </is>
+      </c>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
           <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
-      <c r="D13" s="5" t="n">
-        <v>0.298823830363826</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>0.4460320834017425</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>0.1624299135759245</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <v>0.5466478119994865</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>18.54205120895979</v>
-      </c>
-      <c r="I13" s="9" t="inlineStr">
-        <is>
-          <t>Voting Regressor</t>
-        </is>
-      </c>
-      <c r="J13" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K13" s="8" t="inlineStr">
-        <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
-        </is>
-      </c>
       <c r="L13" s="8" t="n">
-        <v>0.3041030030980708</v>
+        <v>0.9001023929977514</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.4628616458927164</v>
+        <v>0.74574881089283</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.1664887444830136</v>
+        <v>0.2741570238492015</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.5514553500493679</v>
+        <v>0.948737262363902</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>18.79166103126847</v>
+        <v>35.70159993671581</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -3851,19 +3851,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.4892008629205747</v>
+        <v>0.4778736212778882</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.578562420910268</v>
+        <v>0.541572230737098</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.2070425534174271</v>
+        <v>0.2434638770643714</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.6994289548771732</v>
+        <v>0.6912840380609755</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>23.61344524462741</v>
+        <v>20.1450228755492</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -3877,23 +3877,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.5648057025291532</v>
+        <v>0.4225929291407527</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.6492633419274551</v>
+        <v>0.5700667199442087</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.2385777415289289</v>
+        <v>0.2177510211102447</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.7515355630501814</v>
+        <v>0.6500714800241222</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>26.03436171341903</v>
+        <v>23.96852211740612</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -3913,19 +3913,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.1609445306645552</v>
+        <v>0.1830296429464532</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3304258523483574</v>
+        <v>0.3519818028443748</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.1207941891859827</v>
+        <v>0.146725761966493</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.4011789259975594</v>
+        <v>0.427819638336593</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>12.61254519098868</v>
+        <v>14.12568963721907</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -3943,19 +3943,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.1418086000230119</v>
+        <v>0.1784773136075354</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.3123990338625053</v>
+        <v>0.3306253189797487</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.1140243715803865</v>
+        <v>0.1361232289766699</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.3765748265922882</v>
+        <v>0.4224657543606764</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>11.88877117530487</v>
+        <v>13.24478120378263</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -5097,23 +5097,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.365314922165244</v>
+        <v>0.8168332897092256</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.5755327633367506</v>
+        <v>0.7885531847141148</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.2079759754581106</v>
+        <v>0.2798468430505199</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.6044128739241447</v>
+        <v>0.9037882991659195</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>23.5627456397627</v>
+        <v>34.14437257673293</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -5127,23 +5127,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.581745115316429</v>
+        <v>1.672519664085124</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.6419669725940144</v>
+        <v>1.21881816611807</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2236978644068834</v>
+        <v>0.4532546963975154</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.7627221743966993</v>
+        <v>1.293259318189946</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>26.48164464390633</v>
+        <v>61.48136307254385</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -5159,53 +5159,53 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.1753837936785407</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.2861391717946234</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.1041525827126397</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.4187884832209939</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>10.89648545857804</v>
+      </c>
+      <c r="I14" s="9" t="inlineStr">
+        <is>
+          <t>Stacking Regressor</t>
+        </is>
+      </c>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
           <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
-      <c r="D14" s="5" t="n">
-        <v>4.720763713019433e-05</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>0.006717598049104405</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0.002422981300482854</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>0.006870781406084342</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>0.241992129716374</v>
-      </c>
-      <c r="I14" s="9" t="inlineStr">
-        <is>
-          <t>Stacking Regressor</t>
-        </is>
-      </c>
-      <c r="J14" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K14" s="8" t="inlineStr">
-        <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
-        </is>
-      </c>
       <c r="L14" s="8" t="n">
-        <v>0.183672142175393</v>
+        <v>0.1307758287964208</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.3594548582677164</v>
+        <v>0.3149424916821614</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.1254557968207901</v>
+        <v>0.1127114038186749</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.4285698801542089</v>
+        <v>0.3616294080912403</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>13.55931658331474</v>
+        <v>11.84246606855576</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -5221,53 +5221,53 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
+          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 0.5}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.2109671537448551</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.4061769413535049</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.1444302439533725</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.4593116085457182</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>15.8803294966672</v>
+      </c>
+      <c r="I15" s="9" t="inlineStr">
+        <is>
+          <t>Gradient Boosting Regressor</t>
+        </is>
+      </c>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
           <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
         </is>
       </c>
-      <c r="D15" s="5" t="n">
-        <v>1.221674782657097</v>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>0.9745545086973095</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>0.3427897129259097</v>
-      </c>
-      <c r="G15" s="5" t="n">
-        <v>1.105293980195811</v>
-      </c>
-      <c r="H15" s="5" t="n">
-        <v>43.94619632136772</v>
-      </c>
-      <c r="I15" s="9" t="inlineStr">
-        <is>
-          <t>Gradient Boosting Regressor</t>
-        </is>
-      </c>
-      <c r="J15" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K15" s="8" t="inlineStr">
-        <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
-        </is>
-      </c>
       <c r="L15" s="8" t="n">
-        <v>0.1042351832356667</v>
+        <v>2.023100707974391</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.2665067924221832</v>
+        <v>1.295905935605292</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.09187252140872537</v>
+        <v>0.4846771410062844</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.3228547401474334</v>
+        <v>1.422357447329746</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>9.810045180283922</v>
+        <v>69.86360736623483</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -6407,23 +6407,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.04518772938308239</v>
+        <v>0.008521886156027456</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1350706316729728</v>
+        <v>0.08169090613465159</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>1.122584378726192</v>
+        <v>0.12853904801278</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.212574056232369</v>
+        <v>0.09231406261251562</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>27.93316521253714</v>
+        <v>13.3942724980776</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -6437,23 +6437,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.04502630938714355</v>
+        <v>0.01428302759478402</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1361421276750732</v>
+        <v>0.0908130795863407</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>1.119873821835027</v>
+        <v>0.1571907015103586</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2121940371149565</v>
+        <v>0.1195116211704285</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>28.10313027142064</v>
+        <v>18.67117297937411</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -6469,23 +6469,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearRegression()}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.05880856099331029</v>
+        <v>0.02511552621143409</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1508807685114685</v>
+        <v>0.1261894605760267</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>1.333706768805495</v>
+        <v>0.1733334955535343</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2425047648878477</v>
+        <v>0.1584787878911058</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>29.40554684619863</v>
+        <v>18.78495645295575</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -6499,23 +6499,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.04822632896635664</v>
+        <v>0.008883112826339579</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.1407135188733756</v>
+        <v>0.07791012846323568</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>1.169236750605633</v>
+        <v>0.1273428274996332</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2196049383924611</v>
+        <v>0.0942502669828557</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>28.59731776014995</v>
+        <v>13.79928728392985</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -6531,53 +6531,53 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.02207473247341578</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.1250322024968341</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.1982198006289326</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.1485756792796714</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>22.24012456584292</v>
+      </c>
+      <c r="I15" s="9" t="inlineStr">
+        <is>
+          <t>Gradient Boosting Regressor</t>
+        </is>
+      </c>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
           <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
         </is>
       </c>
-      <c r="D15" s="5" t="n">
-        <v>0.05469914907994643</v>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>0.163225448513778</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>1.157665406759229</v>
-      </c>
-      <c r="G15" s="5" t="n">
-        <v>0.2338784921277423</v>
-      </c>
-      <c r="H15" s="5" t="n">
-        <v>31.8759429626266</v>
-      </c>
-      <c r="I15" s="9" t="inlineStr">
-        <is>
-          <t>Gradient Boosting Regressor</t>
-        </is>
-      </c>
-      <c r="J15" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K15" s="8" t="inlineStr">
-        <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
-        </is>
-      </c>
       <c r="L15" s="8" t="n">
-        <v>0.0488284034908474</v>
+        <v>0.005336168169881928</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1657965816321791</v>
+        <v>0.05737232408732598</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>1.055525925735141</v>
+        <v>0.09709931846161093</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.220971499272751</v>
+        <v>0.07304908055466494</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>33.15216354881628</v>
+        <v>10.45765939282463</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -7717,23 +7717,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.03697803078280751</v>
+        <v>0.004274272603528408</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1149609947764105</v>
+        <v>0.05542250340059231</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>1.090379880213352</v>
+        <v>0.09477138382583337</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1922967258764629</v>
+        <v>0.06537792137662689</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>24.68918158688493</v>
+        <v>9.442449699880306</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -7747,23 +7747,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.03726720225693014</v>
+        <v>0.006640108041810892</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.116032276059718</v>
+        <v>0.06253021256703739</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>1.093874294507128</v>
+        <v>0.1120332906990662</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1930471503465672</v>
+        <v>0.08148685809264518</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>24.83413520025046</v>
+        <v>11.08512453143212</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -7779,23 +7779,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.06615452949701239</v>
+        <v>0.04273982076862778</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1976129727979353</v>
+        <v>0.1818134821306851</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>1.324155050136686</v>
+        <v>0.3586383278739438</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2572052283625129</v>
+        <v>0.2067361138471646</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>37.13365773700935</v>
+        <v>29.40422850809043</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -7809,23 +7809,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearRegression()}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.07148399845264874</v>
+        <v>0.05131566841295315</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2060604091058319</v>
+        <v>0.1994302536333513</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>1.371524450869871</v>
+        <v>0.4015396980759681</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2673649162710933</v>
+        <v>0.2265296192839982</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>38.17183469246847</v>
+        <v>31.74462415633885</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -7841,23 +7841,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.04251208628999208</v>
+        <v>0.006982964478830077</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1393287820422499</v>
+        <v>0.06311637904828757</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>1.182448937277118</v>
+        <v>0.1058340150752054</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2061845927560837</v>
+        <v>0.08356413392616521</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>28.44174635548774</v>
+        <v>11.56993071411507</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -7871,23 +7871,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.04234921811748574</v>
+        <v>0.004495853626442241</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1385165037149908</v>
+        <v>0.05641152075169759</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>1.176930211372201</v>
+        <v>0.09694886607755539</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2057892565647822</v>
+        <v>0.06705112695877856</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>28.2780869693781</v>
+        <v>9.632822275313732</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -9027,23 +9027,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.03456650123834975</v>
+        <v>0.01490323323505413</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.103294349452084</v>
+        <v>0.08966208484173777</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>1.155160222227955</v>
+        <v>0.2445579834914141</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1859206853428358</v>
+        <v>0.1220787992857651</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>22.30432872805093</v>
+        <v>17.41458033882164</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -9057,23 +9057,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.03519354950333243</v>
+        <v>0.01342235787652841</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.09701042705985552</v>
+        <v>0.08580159308928278</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>1.175093545987445</v>
+        <v>0.2229076441004665</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1875994389739277</v>
+        <v>0.1158549000971837</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>20.90327206845607</v>
+        <v>16.59126550913074</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -9093,19 +9093,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.04234172711372365</v>
+        <v>0.02766153143839479</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1288196149979995</v>
+        <v>0.1301592587347807</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>1.202058239706559</v>
+        <v>0.3604687949401064</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2057710550921185</v>
+        <v>0.166317562026368</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>26.62076092318772</v>
+        <v>23.63326433390976</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -9123,19 +9123,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.09168976926685395</v>
+        <v>0.05900776614844484</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2644861980735655</v>
+        <v>0.1880870391308913</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>1.375542819432341</v>
+        <v>0.4267654195564308</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.3028031856946917</v>
+        <v>0.2429151418673707</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>44.83537400990734</v>
+        <v>33.00803390835296</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -9151,23 +9151,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.03656481490511735</v>
+        <v>0.01655779985337032</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1258862364846473</v>
+        <v>0.08488106152221278</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>1.112488508000285</v>
+        <v>0.2860562053737314</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.1912192848671842</v>
+        <v>0.1286771147227444</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>27.13678184192788</v>
+        <v>17.00409923112513</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -9181,23 +9181,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.01877592111511714</v>
+        <v>0.01748279799860811</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.0975987227971848</v>
+        <v>0.09593754302789091</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.7774019066756872</v>
+        <v>0.2769700789269216</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.1370252572160225</v>
+        <v>0.1322225321138879</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>22.03298251685202</v>
+        <v>18.51031263092164</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -10341,19 +10341,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.512300125163881</v>
+        <v>0.05232499287216336</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.3380873598932171</v>
+        <v>0.1900034561295903</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.5774723851576025</v>
+        <v>0.07016654470979207</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.7157514409093991</v>
+        <v>0.2287465690937535</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>17.01486445408287</v>
+        <v>7.322671135855377</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -10367,23 +10367,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.5133574082627403</v>
+        <v>0.05791007555769215</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.3403186507779192</v>
+        <v>0.196214499358535</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.5784125475944646</v>
+        <v>0.0719171296678448</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.7164896428160985</v>
+        <v>0.2406451236939825</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>17.10007339547975</v>
+        <v>7.561144212832454</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -10399,23 +10399,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.5517076377949701</v>
+        <v>0.04201193720820822</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.3596372409408285</v>
+        <v>0.1434654914037453</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.5881549754922859</v>
+        <v>0.04966391164573731</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.7427702456311576</v>
+        <v>0.2049681370560025</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>17.76587239244833</v>
+        <v>5.188387142459163</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -10429,23 +10429,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.5537345272717408</v>
+        <v>0.04464348456876042</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.3832909180503301</v>
+        <v>0.1748451014655653</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.5949683290521423</v>
+        <v>0.06181596735366129</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.7441334069047973</v>
+        <v>0.2112900484375931</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>18.70490542474536</v>
+        <v>6.30849117509302</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -10461,23 +10461,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.586678559593703</v>
+        <v>0.07743529926871474</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.4219335040964415</v>
+        <v>0.2391866902385677</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.5990661342283035</v>
+        <v>0.08436349887004509</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.7659494497639534</v>
+        <v>0.2782719879339542</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>19.9725994533928</v>
+        <v>8.909773259342687</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -10491,23 +10491,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.5148254822795786</v>
+        <v>0.04338382901785041</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.3669591049170592</v>
+        <v>0.1697487714205255</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.5698671012546762</v>
+        <v>0.06073933052931837</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.7175134021602514</v>
+        <v>0.2082878513448406</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>18.14541939060312</v>
+        <v>6.364171388961094</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -11647,53 +11647,53 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.1159025241853091</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.2082927780942238</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.0814289499023895</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.3404445978207161</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>8.698558717858971</v>
+      </c>
+      <c r="I13" s="9" t="inlineStr">
+        <is>
+          <t>Voting Regressor</t>
+        </is>
+      </c>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
           <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
-      <c r="D13" s="5" t="n">
-        <v>0.4501396261498773</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>0.2890083119887313</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>0.5592838810304112</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <v>0.6709244563658991</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>15.16190601998442</v>
-      </c>
-      <c r="I13" s="9" t="inlineStr">
-        <is>
-          <t>Voting Regressor</t>
-        </is>
-      </c>
-      <c r="J13" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K13" s="8" t="inlineStr">
-        <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
-        </is>
-      </c>
       <c r="L13" s="8" t="n">
-        <v>0.4610386949842923</v>
+        <v>0.07165440525330201</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.2944542437448597</v>
+        <v>0.1951085587081074</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.5636891207031072</v>
+        <v>0.08386107231757003</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.678998302637269</v>
+        <v>0.2676834048896233</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>15.39304796532981</v>
+        <v>8.07752701462895</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -11713,19 +11713,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.529602467528693</v>
+        <v>0.2691183229359131</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.3450070288864111</v>
+        <v>0.3856717074394787</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.6044277395204345</v>
+        <v>0.1635306516371913</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.7277379112899732</v>
+        <v>0.518766154385493</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>17.11465762646768</v>
+        <v>15.56615179225501</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -11743,19 +11743,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.4377352690557804</v>
+        <v>0.1050629601802968</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2873694313928031</v>
+        <v>0.1910430972877119</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.5512952057807969</v>
+        <v>0.0941802761714253</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.6616156505523281</v>
+        <v>0.3241341700288582</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>15.17259121157782</v>
+        <v>7.903212578491554</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -11771,23 +11771,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.4454202453683997</v>
+        <v>0.1568641888995582</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3190332621292165</v>
+        <v>0.3272886563244938</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.5524275938106595</v>
+        <v>0.1324652639125962</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.6673981160959325</v>
+        <v>0.3960608398965469</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>16.38687069806565</v>
+        <v>13.14032090271475</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -11801,23 +11801,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.4761610323984266</v>
+        <v>0.1353023990088567</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.305519023226616</v>
+        <v>0.2984344782333951</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.5688254082288448</v>
+        <v>0.1233583938101826</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.690044224958391</v>
+        <v>0.3678347441567432</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>15.78889852984139</v>
+        <v>11.97904818573976</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -12957,23 +12957,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.2991143068154603</v>
+        <v>0.09621402797193596</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.2181328546813191</v>
+        <v>0.2035910794712417</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.2103242969981158</v>
+        <v>0.1192516520389258</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.5469134363091295</v>
+        <v>0.3101838615594563</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>11.50198758009906</v>
+        <v>9.495984142279678</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -12987,23 +12987,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.3038478538090966</v>
+        <v>0.08224946188790085</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.209082573717807</v>
+        <v>0.2087039983653424</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2087196851960877</v>
+        <v>0.0965558345532625</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.5512239597560111</v>
+        <v>0.2867916698370105</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>11.08170045860897</v>
+        <v>9.148666016052248</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -13019,23 +13019,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.5843619854227883</v>
+        <v>0.1849848985741422</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.4809989977797297</v>
+        <v>0.2275097695878177</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.3573975513579988</v>
+        <v>0.1609101217936854</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.7644357300798991</v>
+        <v>0.4300987079428886</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>21.93775293683774</v>
+        <v>10.56569093125527</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -13049,23 +13049,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.4601658435280719</v>
+        <v>0.201636890451286</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.3407287654444687</v>
+        <v>0.2783881603542653</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.2940911622821892</v>
+        <v>0.1756098350446483</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.6783552487657717</v>
+        <v>0.4490399653163246</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>16.78450173643841</v>
+        <v>12.43273488142659</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -13081,23 +13081,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.3863765405650877</v>
+        <v>0.1810393877320447</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3551137754308286</v>
+        <v>0.3370884986676313</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2780125670806696</v>
+        <v>0.1771346403621261</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.6215919405567351</v>
+        <v>0.4254872356863889</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>17.01361352847776</v>
+        <v>14.75598238845269</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -13111,23 +13111,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.3621774375158033</v>
+        <v>0.2062774543528318</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.2843820032291012</v>
+        <v>0.3486169906187808</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.2415115607317084</v>
+        <v>0.1820149658644146</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.6018117957599396</v>
+        <v>0.4541777783564843</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>14.13229428888049</v>
+        <v>15.22993190991346</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -14177,23 +14177,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.02918288076536792</v>
+        <v>0.01490378820710876</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1319724205745226</v>
+        <v>0.09798033408731549</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1830856499584939</v>
+        <v>0.1546681558186334</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1708299761908545</v>
+        <v>0.1220810722721125</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>19.69849433257551</v>
+        <v>14.19391013092403</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -14221,23 +14221,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.01256920090042126</v>
+        <v>0.1484920796523707</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.081846952895773</v>
+        <v>0.2375545026932952</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1035718645634325</v>
+        <v>0.2957347602431422</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.1121124475712722</v>
+        <v>0.385346700585811</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>11.08419695709485</v>
+        <v>46.09700787243847</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -14265,23 +14265,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.03702627728318406</v>
+        <v>0.01125698755778994</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1606033739976293</v>
+        <v>0.0898269687463689</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.221576967673556</v>
+        <v>0.1375229203292425</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.1924221330387543</v>
+        <v>0.1060989517280446</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>23.54096596972398</v>
+        <v>13.7911384129736</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -15289,23 +15289,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.01039753791048263</v>
+        <v>0.01177382159407431</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.07846827972353053</v>
+        <v>0.08617046645511338</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1218866290293</v>
+        <v>0.2065769100493164</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1019683181703152</v>
+        <v>0.1085072421273083</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>13.05591444961765</v>
+        <v>16.80536096864774</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -15319,23 +15319,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.00982740225619135</v>
+        <v>0.0133963010160595</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.07410219044382896</v>
+        <v>0.09686884823651193</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.1176080225524245</v>
+        <v>0.2234755025585314</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.09913325504688802</v>
+        <v>0.1157423907479861</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>12.51745254159851</v>
+        <v>18.41926241762036</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -15355,19 +15355,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.01625908191257938</v>
+        <v>0.03024249763107714</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.09639158546728442</v>
+        <v>0.1266138478319371</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1486961111150705</v>
+        <v>0.3705165544736278</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.1275111050559103</v>
+        <v>0.173903702177605</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>15.46619190157567</v>
+        <v>22.8008725133358</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -15385,19 +15385,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.01368689161603501</v>
+        <v>0.02797275631620079</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.09613202154926694</v>
+        <v>0.1225885261603617</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.2192599318108107</v>
+        <v>0.3196750739907355</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.1169909894651507</v>
+        <v>0.1672505794196265</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>16.80107637707817</v>
+        <v>22.11532160444509</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -15413,23 +15413,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.04559795776748539</v>
+        <v>0.03376009352659107</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1683084737137323</v>
+        <v>0.1469058710131005</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.3388445163446789</v>
+        <v>0.415463584836827</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2135367831720928</v>
+        <v>0.1837391997549545</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>27.48760837373078</v>
+        <v>26.46021264400427</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -15443,23 +15443,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.01262505142202097</v>
+        <v>0.03376009352659107</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.08608138250940178</v>
+        <v>0.1469058710131005</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.1537930880388131</v>
+        <v>0.415463584836827</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.1123612540959782</v>
+        <v>0.1837391997549545</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>14.92618634175118</v>
+        <v>26.46021264400427</v>
       </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
@@ -16509,23 +16509,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.0388621023495786</v>
+        <v>0.04683152132390502</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1526901361531687</v>
+        <v>0.165758665624973</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.2151427995328935</v>
+        <v>0.3466207878743333</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1971347314644951</v>
+        <v>0.2164059179502839</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>24.01044985305289</v>
+        <v>32.28085213476013</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -16557,19 +16557,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.02483120411762342</v>
+        <v>0.008001959458530581</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1234536899166371</v>
+        <v>0.07764059216775412</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.179004152584723</v>
+        <v>0.1302078939328934</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.1575791995081312</v>
+        <v>0.08945367213552824</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>19.18150851160172</v>
+        <v>13.42552579120245</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -16597,23 +16597,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.03928414133125136</v>
+        <v>0.01236935988357631</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1583265539750578</v>
+        <v>0.08912626381066661</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2457944690059714</v>
+        <v>0.1502751566037693</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.1982022737792162</v>
+        <v>0.1112176239791891</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>24.28600248719698</v>
+        <v>16.45830389569397</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -17531,23 +17531,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.2350969807814074</v>
+        <v>0.01384565120125302</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.3560071661682788</v>
+        <v>0.09631010685175755</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.8373239657332032</v>
+        <v>0.215406107036712</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.4848680034621871</v>
+        <v>0.1176675452333949</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>61.06527278184863</v>
+        <v>17.47039021476285</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -17579,19 +17579,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.04772958293475262</v>
+        <v>0.01775020334633183</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1402240735617497</v>
+        <v>0.1046612736807838</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.3196834112623548</v>
+        <v>0.3012199429955941</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2184710116577314</v>
+        <v>0.1332298890877412</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>27.19210656908103</v>
+        <v>20.11301670157347</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -17619,23 +17619,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.030506850871355</v>
+        <v>0.04220703276553919</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1346531749434235</v>
+        <v>0.1626438503729845</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2279042553792247</v>
+        <v>0.4110356888449695</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.1746621048520686</v>
+        <v>0.2054435026121274</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>21.21404617536519</v>
+        <v>28.81331172743967</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -18553,23 +18553,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.2187280210969364</v>
+        <v>1.326742380919571</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.3945805787532696</v>
+        <v>0.7769944769379918</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.140681369135949</v>
+        <v>0.2877220500834361</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.4676836763207974</v>
+        <v>1.151843036580753</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>15.2174592603724</v>
+        <v>41.42736857934327</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -18601,19 +18601,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.04646250168212166</v>
+        <v>0.05650631814417815</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1426325563168261</v>
+        <v>0.1802099797357656</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.05352272748645187</v>
+        <v>0.06745407142135534</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2155516218498985</v>
+        <v>0.2377105764247316</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>5.077290384366648</v>
+        <v>6.561282379571942</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -18641,23 +18641,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.15206400279622</v>
+        <v>0.109380371317124</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3273701122728627</v>
+        <v>0.2748591771688831</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.113027945556421</v>
+        <v>0.09746173493715324</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.3899538470078479</v>
+        <v>0.330727034451561</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>12.25706666684981</v>
+        <v>10.4499142107113</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -19575,23 +19575,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>1.540978086383506</v>
+        <v>1.840362084334883</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.9409476173970628</v>
+        <v>1.229216231320612</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.3472088168117737</v>
+        <v>0.4641024828788241</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>1.241361384280784</v>
+        <v>1.356599456116242</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>49.56537136607139</v>
+        <v>55.92419966467964</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -19623,19 +19623,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.4398958848315898</v>
+        <v>0.15297211288377</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.4677972533175891</v>
+        <v>0.2713110995205569</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1826674573006138</v>
+        <v>0.1260118206808305</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.6632464736669089</v>
+        <v>0.3911164952846786</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>15.46618955737363</v>
+        <v>10.81793897525345</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -19667,19 +19667,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.1448935197637982</v>
+        <v>0.1966035733933567</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3181432473751586</v>
+        <v>0.3579937043985228</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.1155263820443957</v>
+        <v>0.1465564017227612</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.3806488142156733</v>
+        <v>0.4434000151030181</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>12.11171506072897</v>
+        <v>14.3805510049068</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -20597,23 +20597,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.3134729283535259</v>
+        <v>1.956840258039265</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.4368753735399066</v>
+        <v>1.142051649968837</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.167450604464088</v>
+        <v>0.5125018704952736</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.5598865316772015</v>
+        <v>1.398871065552242</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>17.99955044513542</v>
+        <v>58.92132999232707</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -20645,19 +20645,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.1250088587423953</v>
+        <v>0.1766363598219773</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2140686780380001</v>
+        <v>0.2454985958598197</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1114080844657333</v>
+        <v>0.1619311361205658</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.3535659185249552</v>
+        <v>0.420281286547447</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>8.998817299921246</v>
+        <v>11.22479395168031</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -20685,23 +20685,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.3106905028158632</v>
+        <v>0.2426356659040417</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.4633730418729498</v>
+        <v>0.3788237551513692</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.1895592590703972</v>
+        <v>0.2028395722328293</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.5573961811995695</v>
+        <v>0.4925806186849435</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>19.08225464139818</v>
+        <v>16.37597444758325</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -21709,23 +21709,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.01154344806255134</v>
+        <v>0.006120192016825021</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.07408747795265137</v>
+        <v>0.06012320962571658</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1061619366314453</v>
+        <v>0.09528537146584415</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1074404396051661</v>
+        <v>0.07823165610432277</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>11.8414854814112</v>
+        <v>10.35388116423032</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -21739,23 +21739,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.01488481689920652</v>
+        <v>0.005535485049966661</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.08839682498063219</v>
+        <v>0.05677321933914242</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.126429986455675</v>
+        <v>0.08995749975391937</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1220033479016315</v>
+        <v>0.07440084038481461</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>14.19252397219208</v>
+        <v>9.476067990538183</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -21775,19 +21775,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.01609552612780798</v>
+        <v>0.01419238802985192</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.09361443961301816</v>
+        <v>0.09330944816521053</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.1438214086839515</v>
+        <v>0.1542796947614722</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.1268681446534471</v>
+        <v>0.1191318094794666</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>13.92351792819716</v>
+        <v>15.46801614530766</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -21805,19 +21805,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.01218098244121581</v>
+        <v>0.02149639031044486</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.0805318969657491</v>
+        <v>0.1180919036049075</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.1152336943088542</v>
+        <v>0.225547638065077</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.1103674881530599</v>
+        <v>0.1466164735302444</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>11.73286624451748</v>
+        <v>19.730291639161</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -21837,19 +21837,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.009067965026057084</v>
+        <v>0.0115446531601238</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.07271949742377345</v>
+        <v>0.08183659604976744</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.1155182753452332</v>
+        <v>0.1235278414180291</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.09522586322033046</v>
+        <v>0.1074460476710233</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>12.47760285238758</v>
+        <v>13.35435489691229</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -21867,19 +21867,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.01981283583215756</v>
+        <v>0.01147360651226855</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1167209868507359</v>
+        <v>0.08757481064033745</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.1677452169885068</v>
+        <v>0.1303919841813123</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.1407580755486433</v>
+        <v>0.1071149219869414</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>18.80152769236199</v>
+        <v>13.72057000228707</v>
       </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
@@ -23019,23 +23019,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.05542053172860058</v>
+        <v>0.1484015136024242</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1760950803293676</v>
+        <v>0.2928022443891146</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.06154417318109934</v>
+        <v>0.1014716580542244</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2354156573565161</v>
+        <v>0.3852291702382158</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>6.454327067704425</v>
+        <v>11.08822643635957</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -23049,23 +23049,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.05858525017000873</v>
+        <v>0.04031788897699198</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.2012602455619599</v>
+        <v>0.1624922484918353</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.07172022125426364</v>
+        <v>0.05795996952053876</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2420439013278557</v>
+        <v>0.2007931497262593</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>7.548484998367848</v>
+        <v>5.975335403858475</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -23085,19 +23085,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.012047551980325</v>
+        <v>0.02421050856555542</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.09107772936118678</v>
+        <v>0.1398620117211604</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.03286254638445667</v>
+        <v>0.05193637354608074</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.1097613410100523</v>
+        <v>0.1555972640040802</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>3.256201557242659</v>
+        <v>5.198864039965541</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -23115,19 +23115,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.02727141392038016</v>
+        <v>0.02690298434878434</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.1239116918605985</v>
+        <v>0.1286633930717154</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.04262797420252511</v>
+        <v>0.04510197621602989</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.1651405883493823</v>
+        <v>0.1640212923640841</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>4.385439164653096</v>
+        <v>4.617394336811712</v>
       </c>
     </row>
     <row r="15" ht="42.75" customHeight="1">
@@ -23147,19 +23147,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.09641839592650238</v>
+        <v>0.1309250492672866</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2592260181448853</v>
+        <v>0.3049085056867895</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.08935557446442141</v>
+        <v>0.1067546114192788</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.3105131171569124</v>
+        <v>0.3618356661072628</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>9.52099333042829</v>
+        <v>11.48689057879469</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -23177,19 +23177,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.06445683550879587</v>
+        <v>0.06070748527242069</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.2064557601909971</v>
+        <v>0.2016293622012748</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.07128383465103959</v>
+        <v>0.0710157808240512</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2538835077526618</v>
+        <v>0.2463888903185789</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>7.508001611718536</v>
+        <v>7.46258531773038</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -24330,23 +24330,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.06795354500436457</v>
+        <v>0.116660816934086</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1688846615911083</v>
+        <v>0.2363404433621184</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.07933859806233318</v>
+        <v>0.1289890640064474</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2606790076020019</v>
+        <v>0.3415564622929656</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>7.170052743495335</v>
+        <v>10.78802194891196</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -24360,23 +24360,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.06707546117167366</v>
+        <v>0.1021131751895863</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1862262760092889</v>
+        <v>0.2374898373367786</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.07766211738542853</v>
+        <v>0.1151076428853305</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2589893070604917</v>
+        <v>0.3195515219641213</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>7.611272989608751</v>
+        <v>10.6183139290415</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -24396,19 +24396,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.1058180778442196</v>
+        <v>0.1869833850773887</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1534321275905388</v>
+        <v>0.2187750490447671</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.08809684933142148</v>
+        <v>0.1602092716799105</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.3252969072158843</v>
+        <v>0.4324157548903471</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>6.789186705739279</v>
+        <v>10.22837080469653</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -24426,19 +24426,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.08866693449978783</v>
+        <v>0.1637798301948524</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.1766978338663119</v>
+        <v>0.2224725381015044</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.08920682230246633</v>
+        <v>0.152618501313846</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2977699355203406</v>
+        <v>0.4046972080393592</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>7.578821308844947</v>
+        <v>10.37401064209875</v>
       </c>
     </row>
     <row r="15" ht="42.75" customHeight="1">
@@ -24458,19 +24458,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.1547414090466067</v>
+        <v>0.1859248209055606</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.317283973611676</v>
+        <v>0.3419177691299968</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.136469152614819</v>
+        <v>0.1793028908656633</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.393371845772682</v>
+        <v>0.4311900055724397</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>12.86234923906378</v>
+        <v>14.95163919695217</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -24484,23 +24484,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.1797099739082123</v>
+        <v>0.1763915165259207</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.3425758109784422</v>
+        <v>0.3315938554321319</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.1472075902793563</v>
+        <v>0.170713512600976</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.4239221318924176</v>
+        <v>0.4199899005046678</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>13.87405228643344</v>
+        <v>14.53758691833625</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -25641,23 +25641,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.0684543802751485</v>
+        <v>0.1868933428939677</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1901071653883977</v>
+        <v>0.3281672395114432</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.06850175802635128</v>
+        <v>0.1350355941504827</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2616378800463505</v>
+        <v>0.4323116270631264</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>7.27016036364603</v>
+        <v>13.39422650794667</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -25675,19 +25675,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.05297114483779598</v>
+        <v>0.2675790430414829</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1615033034045295</v>
+        <v>0.3268544558836162</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.0585836775225524</v>
+        <v>0.1306883217455523</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2301546107246083</v>
+        <v>0.5172804297878308</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>6.054467265764933</v>
+        <v>14.66356348281466</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -25707,19 +25707,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.0333370969771663</v>
+        <v>0.1030686807528391</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.09773503032370742</v>
+        <v>0.1819820423262151</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.0425811832420449</v>
+        <v>0.09223508037685113</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.1825844927072568</v>
+        <v>0.3210431135421519</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>3.893808493847143</v>
+        <v>7.618499652777773</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -25737,19 +25737,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.03709078409452823</v>
+        <v>0.09911373436396925</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.1336559414593915</v>
+        <v>0.2078738251838681</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.05311694377558381</v>
+        <v>0.09624469877623751</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.1925896780581146</v>
+        <v>0.3148233383406784</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>5.125771796723582</v>
+        <v>8.435243559158796</v>
       </c>
     </row>
     <row r="15" ht="42.75" customHeight="1">
@@ -25769,19 +25769,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.1032605258212097</v>
+        <v>0.199345092056154</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2786278701887796</v>
+        <v>0.3629362816476941</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.1010206167250612</v>
+        <v>0.1499021705789642</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.3213417586016635</v>
+        <v>0.4464807857636809</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>10.5406572771299</v>
+        <v>14.560217686284</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -25795,23 +25795,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.07411274171138367</v>
+        <v>0.1320598406434556</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.232422227830839</v>
+        <v>0.2984475980667086</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.08815242654466753</v>
+        <v>0.1229455275867466</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2722365546934938</v>
+        <v>0.3634003861355345</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>8.816784349695979</v>
+        <v>11.9672777519537</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -26954,53 +26954,53 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.04510068155552985</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.1689503320250498</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.226297709256333</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.2123692104697144</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>26.89149481770562</v>
+      </c>
+      <c r="I13" s="9" t="inlineStr">
+        <is>
+          <t>Voting Regressor</t>
+        </is>
+      </c>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
           <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
-      <c r="D13" s="5" t="n">
-        <v>0.03241712192752679</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>0.1342791651316924</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>0.1728802993271292</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <v>0.1800475546280115</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>20.00104670333702</v>
-      </c>
-      <c r="I13" s="9" t="inlineStr">
-        <is>
-          <t>Voting Regressor</t>
-        </is>
-      </c>
-      <c r="J13" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K13" s="8" t="inlineStr">
-        <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
-        </is>
-      </c>
       <c r="L13" s="8" t="n">
-        <v>0.03662233276774005</v>
+        <v>0.04980672538492718</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1528442124385878</v>
+        <v>0.1826987865635949</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.1969216328046443</v>
+        <v>0.2494785646279711</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1913696234195491</v>
+        <v>0.2231742041207433</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>22.75134765940671</v>
+        <v>29.81777350865247</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -27016,23 +27016,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearRegression()}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>6.756136051202942e-05</v>
+        <v>0.04734318653455403</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.006788202926610178</v>
+        <v>0.1809559602594187</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.008800961742363828</v>
+        <v>0.3022055021748114</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.008219571796147863</v>
+        <v>0.217584895005499</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>0.8844635168971907</v>
+        <v>26.23939086817073</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -27046,23 +27046,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.164790672844123</v>
+        <v>0.03134674289066167</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.3343087536559027</v>
+        <v>0.1364561230918045</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.4591379233769612</v>
+        <v>0.2387270627706315</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.40594417454143</v>
+        <v>0.1770501140656556</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>56.49857134269658</v>
+        <v>19.88786515733954</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -27078,23 +27078,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.05294789140659416</v>
+        <v>0.03009849899976461</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1847045617361555</v>
+        <v>0.1370046881753148</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2637856389990065</v>
+        <v>0.1892574314921693</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2301040882005232</v>
+        <v>0.1734891898642812</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>25.87243823564403</v>
+        <v>20.50390236577407</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -27108,23 +27108,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.04406089955204358</v>
+        <v>0.03009849899976461</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1742131448120607</v>
+        <v>0.1370046881753148</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.2276154659966421</v>
+        <v>0.1892574314921693</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2099068830506603</v>
+        <v>0.1734891898642812</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>26.36137293529699</v>
+        <v>20.50390236577407</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -28268,53 +28268,53 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.05270463853997142</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.1768179029561048</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.4152475153272641</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.2295749083414201</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>31.00075962721473</v>
+      </c>
+      <c r="I13" s="9" t="inlineStr">
+        <is>
+          <t>Voting Regressor</t>
+        </is>
+      </c>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
           <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
-      <c r="D13" s="5" t="n">
-        <v>0.0337529644539025</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>0.1363119585277916</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>0.2601056074628622</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <v>0.1837197987531624</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>22.23626139533787</v>
-      </c>
-      <c r="I13" s="9" t="inlineStr">
-        <is>
-          <t>Voting Regressor</t>
-        </is>
-      </c>
-      <c r="J13" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K13" s="8" t="inlineStr">
-        <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
-        </is>
-      </c>
       <c r="L13" s="8" t="n">
-        <v>0.03586413028548839</v>
+        <v>0.04955204633419538</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1401630246912675</v>
+        <v>0.183877216237759</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2543586787540389</v>
+        <v>0.3922894595330763</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1893782730027085</v>
+        <v>0.22260288932131</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>22.932375229108</v>
+        <v>32.49476226594242</v>
       </c>
     </row>
     <row r="14">
@@ -28334,19 +28334,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.1399302852979218</v>
+        <v>0.08467267442176515</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.3187068685555481</v>
+        <v>0.218586908435852</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.7270631225166623</v>
+        <v>0.7514200382554901</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.3740725668876585</v>
+        <v>0.2909856945311318</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>49.60254184220145</v>
+        <v>34.89998388921008</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -28360,23 +28360,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.1883111322637764</v>
+        <v>0.08586753049346654</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.3722620667351177</v>
+        <v>0.2412027557516552</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.8544745343992631</v>
+        <v>0.7266334000069489</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.4339483059809963</v>
+        <v>0.2930316202962857</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>58.23449872182947</v>
+        <v>38.93649271454672</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -28392,23 +28392,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.05016420995472174</v>
+        <v>0.05358482875635333</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1779620615006171</v>
+        <v>0.1847798958405945</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.3714125642462172</v>
+        <v>0.4966655473809958</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2239736813885099</v>
+        <v>0.2314839708410786</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>28.92868340338037</v>
+        <v>31.88538746614789</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -28422,23 +28422,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.05016420995472174</v>
+        <v>0.05358482875635333</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1779620615006171</v>
+        <v>0.1847798958405945</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.3714125642462172</v>
+        <v>0.4966655473809958</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2239736813885099</v>
+        <v>0.2314839708410786</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>28.92868340338037</v>
+        <v>31.88538746614789</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -29580,23 +29580,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.01656644379705167</v>
+        <v>0.04947930157654035</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1058572434508086</v>
+        <v>0.1817546364939273</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.1655548408219376</v>
+        <v>0.2921213627559956</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.1287106980676108</v>
+        <v>0.2224394335016621</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>16.16472218678046</v>
+        <v>31.45306198742186</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -29614,19 +29614,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.02183179938159012</v>
+        <v>0.04300863241599255</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1269535673126922</v>
+        <v>0.1680454157803269</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.2030699605249353</v>
+        <v>0.294614888559351</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.1477558776549688</v>
+        <v>0.207385227091981</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>19.95466545237592</v>
+        <v>28.18884424166663</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -29646,19 +29646,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.4873622580206562</v>
+        <v>0.285171002115983</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.5594951773469929</v>
+        <v>0.4719016840294443</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.9074878492009186</v>
+        <v>0.9351071217462961</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.6981133561397148</v>
+        <v>0.5340140467403296</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>92.73522264170536</v>
+        <v>87.00379994416706</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -29672,23 +29672,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearRegression()}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.6716682042513148</v>
+        <v>0.0940508755751939</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.6726590938199354</v>
+        <v>0.2622153317615985</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>1.101248612038371</v>
+        <v>0.608118105608224</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.8195536616057028</v>
+        <v>0.3066771520266776</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>105.6512102179655</v>
+        <v>39.64555375316041</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -29704,23 +29704,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.03376053676883926</v>
+        <v>0.04179045613419914</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1510353020263334</v>
+        <v>0.1639137618272858</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.2730909104790326</v>
+        <v>0.3302368526445421</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.1837404059232461</v>
+        <v>0.2044271413834257</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>23.05636575127964</v>
+        <v>27.1309544457224</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -29734,23 +29734,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.02608151821313694</v>
+        <v>0.04179045613419914</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1360944171986248</v>
+        <v>0.1639137618272858</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.2352322169106514</v>
+        <v>0.3302368526445421</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.1614977343901051</v>
+        <v>0.2044271413834257</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>21.2209750850194</v>
+        <v>27.1309544457224</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">

</xml_diff>